<commit_message>
Manuscrito tema 2 con corrección de estilo
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion02/SolicitudGrafica-MA_11_02_CO.xlsx
@@ -1018,9 +1018,6 @@
     <t xml:space="preserve">Grafica de la funcion                                                                                                             con asintotas en x=-3 y x+2 de color rojo con sus respectivas etiquetas.                                                                                                                      </t>
   </si>
   <si>
-    <t>Grafica de la funcion con asintota punteada en y=3 y sus respectivas etiquetas.</t>
-  </si>
-  <si>
     <t>Grafica de la funcion</t>
   </si>
   <si>
@@ -1103,6 +1100,9 @@
   </si>
   <si>
     <t>No se si la imagen sea libre, es mejor hacer una similar.</t>
+  </si>
+  <si>
+    <t>Grafica de la funcion con asintota punteada en y=3 y sus respectivas etiquetas, la funcion es     f(x)=(3x^2-5x+7)/(x^2-1)</t>
   </si>
 </sst>
 </file>
@@ -1847,7 +1847,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2076,6 +2076,15 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2160,14 +2169,8 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -4888,71 +4891,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>750795</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1687046</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>1112745</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="73" name="Imagen 72"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
-          <a:clrChange>
-            <a:clrFrom>
-              <a:srgbClr val="FFFFFF"/>
-            </a:clrFrom>
-            <a:clrTo>
-              <a:srgbClr val="FFFFFF">
-                <a:alpha val="0"/>
-              </a:srgbClr>
-            </a:clrTo>
-          </a:clrChange>
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="20439530" y="103363060"/>
-          <a:ext cx="1362075" cy="361950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -4972,7 +4910,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId49">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5021,7 +4959,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId50">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5086,7 +5024,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId51">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5149,7 +5087,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId52"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5187,7 +5125,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId53">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5250,7 +5188,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId54">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5299,7 +5237,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId55">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5362,7 +5300,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId56">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5409,7 +5347,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId57">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5456,7 +5394,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId58">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5503,7 +5441,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId59">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5552,7 +5490,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId60">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5615,7 +5553,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId61">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5662,7 +5600,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId62">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -5711,7 +5649,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId63">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -5776,7 +5714,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId65">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId64">
           <a:clrChange>
             <a:clrFrom>
               <a:srgbClr val="FFFFFF"/>
@@ -6538,9 +6476,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:G3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -6578,14 +6516,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="F2" s="86" t="s">
+      <c r="D2" s="97"/>
+      <c r="F2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="87"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="44"/>
       <c r="I2" s="44"/>
       <c r="J2" s="16"/>
@@ -6595,12 +6533,12 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="95">
+      <c r="C3" s="98">
         <v>11</v>
       </c>
-      <c r="D3" s="96"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
+      <c r="D3" s="99"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
       <c r="H3" s="44"/>
       <c r="I3" s="44"/>
       <c r="J3" s="16"/>
@@ -6610,10 +6548,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="98" t="s">
         <v>154</v>
       </c>
-      <c r="D4" s="96"/>
+      <c r="D4" s="99"/>
       <c r="E4" s="5"/>
       <c r="F4" s="43" t="s">
         <v>55</v>
@@ -6631,10 +6569,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="100" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="98"/>
+      <c r="D5" s="101"/>
       <c r="E5" s="5"/>
       <c r="F5" s="41" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -6685,12 +6623,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="90" t="s">
+      <c r="F8" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="91"/>
-      <c r="H8" s="91"/>
-      <c r="I8" s="92"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -8553,7 +8491,7 @@
         <v>274</v>
       </c>
       <c r="K57" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="12" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -8593,7 +8531,7 @@
         <v>273</v>
       </c>
       <c r="K58" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="12" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8746,8 +8684,8 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J62" s="14"/>
-      <c r="K62" s="83" t="s">
-        <v>279</v>
+      <c r="K62" s="120" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="12" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8785,7 +8723,7 @@
       </c>
       <c r="J63" s="14"/>
       <c r="K63" s="74" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="12" customFormat="1" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8822,7 +8760,7 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J64" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K64"/>
     </row>
@@ -8861,7 +8799,7 @@
       </c>
       <c r="J65"/>
       <c r="K65" s="74" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:11" s="12" customFormat="1" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8899,7 +8837,7 @@
       </c>
       <c r="J66" s="68"/>
       <c r="K66" s="74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="12" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9013,7 +8951,7 @@
       </c>
       <c r="J69"/>
       <c r="K69" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="12" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
@@ -9051,7 +8989,7 @@
       </c>
       <c r="J70" s="14"/>
       <c r="K70" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="71" spans="1:11" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
@@ -9089,7 +9027,7 @@
       </c>
       <c r="J71" s="14"/>
       <c r="K71" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="12" customFormat="1" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9202,10 +9140,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J74" s="83" t="s">
+        <v>285</v>
+      </c>
+      <c r="K74" s="84" t="s">
         <v>286</v>
-      </c>
-      <c r="K74" s="84" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="75" spans="1:11" ht="171" customHeight="1" x14ac:dyDescent="0.25">
@@ -9243,7 +9181,7 @@
       </c>
       <c r="J75" s="73"/>
       <c r="K75" s="85" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9280,10 +9218,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J76" s="84" t="s">
+        <v>290</v>
+      </c>
+      <c r="K76" s="86" t="s">
         <v>291</v>
-      </c>
-      <c r="K76" s="117" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="87" customHeight="1" x14ac:dyDescent="0.25">
@@ -9320,10 +9258,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J77" t="s">
+        <v>292</v>
+      </c>
+      <c r="K77" s="73" t="s">
         <v>293</v>
-      </c>
-      <c r="K77" s="73" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9360,10 +9298,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J78" s="73" t="s">
+        <v>294</v>
+      </c>
+      <c r="K78" s="73" t="s">
         <v>295</v>
-      </c>
-      <c r="K78" s="73" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9400,10 +9338,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J79" s="84" t="s">
+        <v>296</v>
+      </c>
+      <c r="K79" s="73" t="s">
         <v>297</v>
-      </c>
-      <c r="K79" s="73" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -9440,10 +9378,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J80" s="84" t="s">
+        <v>298</v>
+      </c>
+      <c r="K80" s="73" t="s">
         <v>299</v>
-      </c>
-      <c r="K80" s="73" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -9480,10 +9418,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J81" s="84" t="s">
+        <v>300</v>
+      </c>
+      <c r="K81" s="73" t="s">
         <v>301</v>
-      </c>
-      <c r="K81" s="73" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -9519,19 +9457,19 @@
         <f>IF(OR(B82&lt;&gt;"",J82&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J82" s="118" t="s">
+      <c r="J82" s="87" t="s">
+        <v>302</v>
+      </c>
+      <c r="K82" s="73" t="s">
         <v>303</v>
-      </c>
-      <c r="K82" s="73" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="B83" s="119" t="s">
-        <v>305</v>
+      <c r="B83" s="88" t="s">
+        <v>304</v>
       </c>
       <c r="C83" s="22" t="str">
         <f t="shared" ref="C83" si="21">IF(OR(B83&lt;&gt;"",J83&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -9560,10 +9498,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J83" s="84" t="s">
+        <v>305</v>
+      </c>
+      <c r="K83" s="73" t="s">
         <v>306</v>
-      </c>
-      <c r="K83" s="73" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="103.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9677,25 +9615,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="103"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
+      <c r="F1" s="106"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="35"/>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="107" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="105"/>
-      <c r="E2" s="106"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
       <c r="F2" s="36"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -9703,11 +9641,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="35"/>
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="112"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="115"/>
       <c r="F3" s="36"/>
       <c r="H3" s="26" t="s">
         <v>18</v>
@@ -9758,11 +9696,11 @@
       <c r="C5" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="113" t="str">
+      <c r="D5" s="116" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>MA_11_01_CO</v>
       </c>
-      <c r="E5" s="114"/>
+      <c r="E5" s="117"/>
       <c r="F5" s="36"/>
       <c r="H5" s="26" t="s">
         <v>22</v>
@@ -9807,12 +9745,12 @@
       <c r="C7" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="99" t="str">
+      <c r="D7" s="102" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_CO.xls</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="103"/>
       <c r="H7" s="26" t="s">
         <v>24</v>
       </c>
@@ -9906,14 +9844,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="102"/>
-      <c r="C13" s="102"/>
-      <c r="D13" s="102"/>
-      <c r="E13" s="102"/>
-      <c r="F13" s="103"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="106"/>
       <c r="I13" s="26" t="s">
         <v>33</v>
       </c>
@@ -9946,12 +9884,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="35"/>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="107" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="E15" s="105"/>
-      <c r="F15" s="106"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="109"/>
       <c r="J15" s="26">
         <v>12</v>
       </c>
@@ -9991,12 +9929,12 @@
       <c r="C17" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="107" t="str">
+      <c r="D17" s="110" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>MA_11_01_REC10</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="109"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="112"/>
       <c r="J17" s="26">
         <v>14</v>
       </c>
@@ -10012,12 +9950,12 @@
       <c r="C18" s="66" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="99" t="str">
+      <c r="D18" s="102" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_MA_11_01_REC10.xls</v>
       </c>
-      <c r="E18" s="99"/>
-      <c r="F18" s="100"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="103"/>
       <c r="J18" s="26">
         <v>15</v>
       </c>
@@ -10409,41 +10347,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="118" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="115" t="s">
+      <c r="B1" s="118" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="118" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="115" t="s">
+      <c r="D1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="115" t="s">
+      <c r="E1" s="118" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="115" t="s">
+      <c r="F1" s="118" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="115" t="s">
+      <c r="G1" s="118" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="115"/>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
       <c r="H2" s="45" t="s">
         <v>65</v>
       </c>

</xml_diff>